<commit_message>
Update Excel files with new data and formatting
Anonymized statistischer-bericht and height/width Excel files.
</commit_message>
<xml_diff>
--- a/column_widths_and_row_heights/height_and_width.xlsx
+++ b/column_widths_and_row_heights/height_and_width.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johr\Temp Documents\GitHub\spreadsheet-data-extractor-paper\examples\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6977DB9-DE20-4047-83A9-B432F11C94F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42933F34-6609-48E4-81BC-E9274123E4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32640" xr2:uid="{9221F4BF-38A7-4932-8EE9-A31027FF732C}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="12645" xr2:uid="{9221F4BF-38A7-4932-8EE9-A31027FF732C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +32,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,148 +410,149 @@
       <selection activeCell="AC30" sqref="AC30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="0.140625" customWidth="1"/>
-    <col min="2" max="2" width="0.28515625" customWidth="1"/>
-    <col min="3" max="3" width="0.42578125" customWidth="1"/>
-    <col min="4" max="4" width="0.5703125" customWidth="1"/>
-    <col min="5" max="5" width="0.7109375" customWidth="1"/>
-    <col min="6" max="7" width="0.85546875" customWidth="1"/>
-    <col min="8" max="8" width="1.140625" customWidth="1"/>
-    <col min="9" max="9" width="1.28515625" customWidth="1"/>
-    <col min="10" max="10" width="1.42578125" customWidth="1"/>
-    <col min="11" max="11" width="1.5703125" customWidth="1"/>
-    <col min="12" max="12" width="1.7109375" customWidth="1"/>
-    <col min="13" max="13" width="1.85546875" customWidth="1"/>
+    <col min="1" max="1" width="0.125" customWidth="1"/>
+    <col min="2" max="2" width="0.25" customWidth="1"/>
+    <col min="3" max="3" width="0.375" customWidth="1"/>
+    <col min="4" max="4" width="0.625" customWidth="1"/>
+    <col min="5" max="5" width="0.75" customWidth="1"/>
+    <col min="6" max="7" width="0.875" customWidth="1"/>
+    <col min="8" max="8" width="1.125" customWidth="1"/>
+    <col min="9" max="9" width="1.25" customWidth="1"/>
+    <col min="10" max="10" width="1.375" customWidth="1"/>
+    <col min="11" max="11" width="1.625" customWidth="1"/>
+    <col min="12" max="12" width="1.75" customWidth="1"/>
+    <col min="13" max="13" width="1.875" customWidth="1"/>
     <col min="14" max="14" width="2" customWidth="1"/>
-    <col min="15" max="15" width="2.140625" customWidth="1"/>
-    <col min="16" max="16" width="2.28515625" customWidth="1"/>
-    <col min="17" max="17" width="2.42578125" customWidth="1"/>
-    <col min="18" max="18" width="2.5703125" customWidth="1"/>
-    <col min="19" max="19" width="2.7109375" customWidth="1"/>
-    <col min="20" max="20" width="2.85546875" customWidth="1"/>
+    <col min="15" max="15" width="2.125" customWidth="1"/>
+    <col min="16" max="16" width="2.25" customWidth="1"/>
+    <col min="17" max="17" width="2.375" customWidth="1"/>
+    <col min="18" max="18" width="2.625" customWidth="1"/>
+    <col min="19" max="19" width="2.75" customWidth="1"/>
+    <col min="20" max="20" width="2.875" customWidth="1"/>
     <col min="21" max="23" width="3" customWidth="1"/>
-    <col min="24" max="24" width="3.140625" customWidth="1"/>
-    <col min="25" max="25" width="3.42578125" customWidth="1"/>
-    <col min="26" max="26" width="3.5703125" customWidth="1"/>
-    <col min="27" max="27" width="3.7109375" customWidth="1"/>
-    <col min="28" max="28" width="3.85546875" customWidth="1"/>
+    <col min="24" max="24" width="3.125" customWidth="1"/>
+    <col min="25" max="25" width="3.375" customWidth="1"/>
+    <col min="26" max="26" width="3.625" customWidth="1"/>
+    <col min="27" max="27" width="3.75" customWidth="1"/>
+    <col min="28" max="28" width="3.875" customWidth="1"/>
     <col min="29" max="30" width="4" customWidth="1"/>
-    <col min="31" max="31" width="4.28515625" customWidth="1"/>
-    <col min="32" max="32" width="4.42578125" customWidth="1"/>
-    <col min="33" max="33" width="4.5703125" customWidth="1"/>
-    <col min="34" max="34" width="4.7109375" customWidth="1"/>
-    <col min="35" max="35" width="4.85546875" customWidth="1"/>
+    <col min="31" max="31" width="4.25" customWidth="1"/>
+    <col min="32" max="32" width="4.375" customWidth="1"/>
+    <col min="33" max="33" width="4.625" customWidth="1"/>
+    <col min="34" max="34" width="4.75" customWidth="1"/>
+    <col min="35" max="35" width="4.875" customWidth="1"/>
     <col min="36" max="36" width="5" customWidth="1"/>
-    <col min="37" max="37" width="5.140625" customWidth="1"/>
-    <col min="38" max="38" width="5.28515625" customWidth="1"/>
-    <col min="39" max="39" width="5.42578125" customWidth="1"/>
-    <col min="40" max="40" width="5.5703125" customWidth="1"/>
-    <col min="41" max="41" width="5.7109375" customWidth="1"/>
-    <col min="42" max="42" width="5.85546875" customWidth="1"/>
+    <col min="37" max="37" width="5.125" customWidth="1"/>
+    <col min="38" max="38" width="5.25" customWidth="1"/>
+    <col min="39" max="39" width="5.375" customWidth="1"/>
+    <col min="40" max="40" width="5.625" customWidth="1"/>
+    <col min="41" max="41" width="5.75" customWidth="1"/>
+    <col min="42" max="42" width="5.875" customWidth="1"/>
     <col min="43" max="43" width="6" customWidth="1"/>
-    <col min="44" max="44" width="6.140625" customWidth="1"/>
-    <col min="45" max="45" width="6.28515625" customWidth="1"/>
-    <col min="46" max="47" width="6.42578125" customWidth="1"/>
-    <col min="48" max="48" width="6.7109375" customWidth="1"/>
-    <col min="49" max="49" width="6.85546875" customWidth="1"/>
+    <col min="44" max="44" width="6.125" customWidth="1"/>
+    <col min="45" max="45" width="6.25" customWidth="1"/>
+    <col min="46" max="47" width="6.375" customWidth="1"/>
+    <col min="48" max="48" width="6.75" customWidth="1"/>
+    <col min="49" max="49" width="6.875" customWidth="1"/>
     <col min="50" max="50" width="7" customWidth="1"/>
-    <col min="51" max="51" width="7.140625" customWidth="1"/>
-    <col min="52" max="52" width="7.28515625" customWidth="1"/>
-    <col min="53" max="53" width="7.42578125" customWidth="1"/>
-    <col min="54" max="54" width="7.5703125" customWidth="1"/>
+    <col min="51" max="51" width="7.125" customWidth="1"/>
+    <col min="52" max="52" width="7.25" customWidth="1"/>
+    <col min="53" max="53" width="7.375" customWidth="1"/>
+    <col min="54" max="54" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:15" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" hidden="1"/>
+    <row r="2" spans="1:15" ht="1.5" customHeight="1">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="2.25" customHeight="1">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="3" customHeight="1">
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="3.75" customHeight="1">
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="4.5" customHeight="1">
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="5.25" customHeight="1">
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="6" customHeight="1">
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="6.75" customHeight="1">
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="7.5" customHeight="1">
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="8.25" customHeight="1">
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="9" customHeight="1">
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:15" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="9.75" customHeight="1">
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="10.5" customHeight="1">
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:15" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="11.25" customHeight="1">
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="12" customHeight="1">
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="16:29" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="16:29" ht="12.75" customHeight="1">
       <c r="P17" s="1"/>
     </row>
-    <row r="18" spans="16:29" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="16:29" ht="13.5" customHeight="1">
       <c r="Q18" s="1"/>
     </row>
-    <row r="19" spans="16:29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="16:29" ht="14.25" customHeight="1">
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="16:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="16:29">
       <c r="S20" s="1"/>
     </row>
-    <row r="21" spans="16:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="16:29" ht="15.75" customHeight="1">
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="16:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="16:29" ht="15.75" customHeight="1">
       <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="16:29" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="16:29" ht="16.5" customHeight="1">
       <c r="V23" s="1"/>
     </row>
-    <row r="24" spans="16:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="16:29" ht="17.25" customHeight="1">
       <c r="W24" s="1"/>
     </row>
-    <row r="25" spans="16:29" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="16:29" ht="18" customHeight="1">
       <c r="X25" s="1"/>
     </row>
-    <row r="26" spans="16:29" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="16:29" ht="18.75" customHeight="1">
       <c r="Y26" s="1"/>
     </row>
-    <row r="27" spans="16:29" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="16:29" ht="19.5" customHeight="1">
       <c r="Z27" s="1"/>
     </row>
-    <row r="28" spans="16:29" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="16:29" ht="20.25" customHeight="1">
       <c r="AA28" s="1"/>
     </row>
-    <row r="29" spans="16:29" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="16:29" ht="21" customHeight="1">
       <c r="AB29" s="1"/>
     </row>
-    <row r="30" spans="16:29" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="16:29" ht="19.5" customHeight="1">
       <c r="AC30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>